<commit_message>
Google Sheets export adjusted for Excel
</commit_message>
<xml_diff>
--- a/arduino_c/read_analog/esp8266_analog_input.xlsx
+++ b/arduino_c/read_analog/esp8266_analog_input.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68324F8-CD7B-41E0-ABC3-AA6B2CCF3035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="3945" yWindow="4050" windowWidth="19800" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -22,53 +31,70 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -85,6 +111,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>reading vs voltage</a:t>
             </a:r>
           </a:p>
@@ -92,9 +119,11 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -102,27 +131,214 @@
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>reading</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
               <c:f>Sheet1!$A$2:$A$27</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>621</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>804</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>909</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1035</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1232</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1458</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1691</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2262</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2525</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2820</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2952</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3013</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3076</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3116</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3168</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3203</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3290</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>925</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>967</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>989</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6B2C-4B42-A866-967ED23D384A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="1113020032"/>
         <c:axId val="1015616128"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1113020032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -144,6 +360,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-US"/>
                   <a:t>voltage</a:t>
                 </a:r>
               </a:p>
@@ -154,7 +371,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -167,10 +384,13 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1015616128"/>
-      </c:catAx>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1015616128"/>
         <c:scaling>
@@ -213,6 +433,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-US"/>
                   <a:t>reading</a:t>
                 </a:r>
               </a:p>
@@ -239,36 +460,32 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1113020032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -285,6 +502,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>reading vs voltage</a:t>
             </a:r>
           </a:p>
@@ -292,9 +510,21 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12854628171478566"/>
+          <c:y val="0.11320754716981132"/>
+          <c:w val="0.81905371828521434"/>
+          <c:h val="0.79514824797843664"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -302,13 +532,20 @@
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>reading</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
           <c:trendline>
-            <c:name/>
             <c:spPr>
               <a:ln w="19050">
                 <a:solidFill>
@@ -319,23 +556,191 @@
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.2271391076115487E-2"/>
+                  <c:y val="-5.515008737115408E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
-            <c:strRef>
+          <c:xVal>
+            <c:numRef>
               <c:f>Sheet1!$A$2:$A$24</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>621</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>804</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>909</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1035</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1232</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1458</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1691</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2262</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2525</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2820</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2952</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3013</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3076</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>925</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>967</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>989</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1022</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BAED-406E-A6E6-FC4E5F48ED8F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="340334728"/>
         <c:axId val="1496083092"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="340334728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -357,6 +762,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-US"/>
                   <a:t>voltage</a:t>
                 </a:r>
               </a:p>
@@ -367,7 +773,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -380,10 +786,13 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1496083092"/>
-      </c:catAx>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1496083092"/>
         <c:scaling>
@@ -426,6 +835,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-US"/>
                   <a:t>reading</a:t>
                 </a:r>
               </a:p>
@@ -452,13 +862,26 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="340334728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.7320444444444445"/>
+          <c:y val="0.38207271260903708"/>
+          <c:w val="0.2235111111111111"/>
+          <c:h val="0.12264674462861953"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -472,16 +895,28 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -498,6 +933,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>voltage vs reading</a:t>
             </a:r>
           </a:p>
@@ -505,9 +941,21 @@
       </c:tx>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12854628171478566"/>
+          <c:y val="0.11320754716981132"/>
+          <c:w val="0.81680927384076996"/>
+          <c:h val="0.72790033321306535"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -515,13 +963,20 @@
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$B$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>voltage</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
           <c:trendline>
-            <c:name/>
             <c:spPr>
               <a:ln w="19050">
                 <a:solidFill>
@@ -532,23 +987,191 @@
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6528783902012248E-2"/>
+                  <c:y val="-2.4065199397245156E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
-            <c:strRef>
+          <c:xVal>
+            <c:numRef>
               <c:f>Sheet1!$A$32:$A$54</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>925</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>967</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>989</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$32:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>621</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>804</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>909</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1035</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1232</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1458</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1691</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2262</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2525</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2820</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2952</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3013</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3076</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3116</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E780-41DE-95C8-EDABB807CBB2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="1159864432"/>
         <c:axId val="1804299240"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1159864432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -570,6 +1193,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-US"/>
                   <a:t>reading</a:t>
                 </a:r>
               </a:p>
@@ -580,7 +1204,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -593,10 +1217,13 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1804299240"/>
-      </c:catAx>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1804299240"/>
         <c:scaling>
@@ -639,6 +1266,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="en-US"/>
                   <a:t>voltage</a:t>
                 </a:r>
               </a:p>
@@ -665,13 +1293,26 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1159864432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.73006666666666653"/>
+          <c:y val="0.31378879526851594"/>
+          <c:w val="0.22104444444444443"/>
+          <c:h val="0.12264674462861953"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -685,16 +1326,24 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -703,9 +1352,15 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="2" name="Chart 1" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -714,7 +1369,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -728,9 +1383,15 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="3" name="Chart 2" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -739,7 +1400,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -753,9 +1414,15 @@
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="4" name="Chart 3" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -764,7 +1431,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -774,7 +1441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -964,24 +1631,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.14"/>
-    <col customWidth="1" min="2" max="2" width="7.29"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,215 +1661,215 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2">
-        <v>28.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1">
-        <v>40.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>155.0</v>
+        <v>155</v>
       </c>
       <c r="B6" s="1">
-        <v>59.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>252.0</v>
+        <v>252</v>
       </c>
       <c r="B7" s="1">
-        <v>89.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>367.0</v>
+        <v>367</v>
       </c>
       <c r="B8" s="1">
-        <v>127.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>447.0</v>
+        <v>447</v>
       </c>
       <c r="B9" s="1">
-        <v>153.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>621.0</v>
+        <v>621</v>
       </c>
       <c r="B10" s="1">
-        <v>210.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>804.0</v>
+        <v>804</v>
       </c>
       <c r="B11" s="1">
-        <v>271.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>909.0</v>
+        <v>909</v>
       </c>
       <c r="B12" s="1">
-        <v>305.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>1035.0</v>
+        <v>1035</v>
       </c>
       <c r="B13" s="1">
-        <v>344.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>1232.0</v>
+        <v>1232</v>
       </c>
       <c r="B14" s="1">
-        <v>409.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>1458.0</v>
+        <v>1458</v>
       </c>
       <c r="B15" s="1">
-        <v>484.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>1691.0</v>
+        <v>1691</v>
       </c>
       <c r="B16" s="1">
-        <v>558.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>1993.0</v>
+        <v>1993</v>
       </c>
       <c r="B17" s="1">
-        <v>655.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>2262.0</v>
+        <v>2262</v>
       </c>
       <c r="B18" s="1">
-        <v>745.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>2525.0</v>
+        <v>2525</v>
       </c>
       <c r="B19" s="1">
-        <v>830.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>2820.0</v>
+        <v>2820</v>
       </c>
       <c r="B20" s="1">
-        <v>925.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>2952.0</v>
+        <v>2952</v>
       </c>
       <c r="B21" s="1">
-        <v>967.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>3013.0</v>
+        <v>3013</v>
       </c>
       <c r="B22" s="1">
-        <v>989.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>3076.0</v>
+        <v>3076</v>
       </c>
       <c r="B23" s="1">
-        <v>1010.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>3116.0</v>
+        <v>3116</v>
       </c>
       <c r="B24" s="1">
-        <v>1022.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>3168.0</v>
+        <v>3168</v>
       </c>
       <c r="B25" s="1">
-        <v>1024.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>3203.0</v>
+        <v>3203</v>
       </c>
       <c r="B26" s="1">
-        <v>1024.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>3290.0</v>
+        <v>3290</v>
       </c>
       <c r="B27" s="1">
-        <v>1024.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -1205,191 +1877,192 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B32" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B33" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B34" s="1">
-        <v>55.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1">
-        <v>96.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="B36" s="1">
-        <v>155.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>89.0</v>
+        <v>89</v>
       </c>
       <c r="B37" s="1">
-        <v>252.0</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>127.0</v>
+        <v>127</v>
       </c>
       <c r="B38" s="1">
-        <v>367.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>153.0</v>
+        <v>153</v>
       </c>
       <c r="B39" s="1">
-        <v>447.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>210.0</v>
+        <v>210</v>
       </c>
       <c r="B40" s="1">
-        <v>621.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>271.0</v>
+        <v>271</v>
       </c>
       <c r="B41" s="1">
-        <v>804.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>305.0</v>
+        <v>305</v>
       </c>
       <c r="B42" s="1">
-        <v>909.0</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>344.0</v>
+        <v>344</v>
       </c>
       <c r="B43" s="1">
-        <v>1035.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>409.0</v>
+        <v>409</v>
       </c>
       <c r="B44" s="1">
-        <v>1232.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>484.0</v>
+        <v>484</v>
       </c>
       <c r="B45" s="1">
-        <v>1458.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>558.0</v>
+        <v>558</v>
       </c>
       <c r="B46" s="1">
-        <v>1691.0</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>655.0</v>
+        <v>655</v>
       </c>
       <c r="B47" s="1">
-        <v>1993.0</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>745.0</v>
+        <v>745</v>
       </c>
       <c r="B48" s="1">
-        <v>2262.0</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>830.0</v>
+        <v>830</v>
       </c>
       <c r="B49" s="1">
-        <v>2525.0</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>2525</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>925.0</v>
+        <v>925</v>
       </c>
       <c r="B50" s="1">
-        <v>2820.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>967.0</v>
+        <v>967</v>
       </c>
       <c r="B51" s="1">
-        <v>2952.0</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>2952</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>989.0</v>
+        <v>989</v>
       </c>
       <c r="B52" s="1">
-        <v>3013.0</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>1010.0</v>
+        <v>1010</v>
       </c>
       <c r="B53" s="1">
-        <v>3076.0</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>3076</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>1022.0</v>
+        <v>1022</v>
       </c>
       <c r="B54" s="1">
-        <v>3116.0</v>
+        <v>3116</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>